<commit_message>
updated time when you updated gear
</commit_message>
<xml_diff>
--- a/holy.xlsx
+++ b/holy.xlsx
@@ -82,15 +82,15 @@
     <t>Exposed</t>
   </si>
   <si>
+    <t>WickedKiss</t>
+  </si>
+  <si>
+    <t>zozrog</t>
+  </si>
+  <si>
     <t>Misha</t>
   </si>
   <si>
-    <t>WickedKiss</t>
-  </si>
-  <si>
-    <t>zozrog</t>
-  </si>
-  <si>
     <t>Yamul</t>
   </si>
   <si>
@@ -121,6 +121,9 @@
     <t>wonderdogman</t>
   </si>
   <si>
+    <t>dennymane</t>
+  </si>
+  <si>
     <t>Mrclutchcakes</t>
   </si>
   <si>
@@ -130,9 +133,6 @@
     <t>Maalinko174</t>
   </si>
   <si>
-    <t>dennymane</t>
-  </si>
-  <si>
     <t>Viellideau</t>
   </si>
   <si>
@@ -229,15 +229,15 @@
     <t>Thorn_Ess</t>
   </si>
   <si>
+    <t>Wicked_Kiss</t>
+  </si>
+  <si>
+    <t>Zozrog</t>
+  </si>
+  <si>
     <t>Mishailia</t>
   </si>
   <si>
-    <t>Wicked_Kiss</t>
-  </si>
-  <si>
-    <t>Zozrog</t>
-  </si>
-  <si>
     <t>Flame_Haze</t>
   </si>
   <si>
@@ -256,6 +256,9 @@
     <t>Hooge</t>
   </si>
   <si>
+    <t>Dennymane</t>
+  </si>
+  <si>
     <t>MrClutchCakes</t>
   </si>
   <si>
@@ -263,9 +266,6 @@
   </si>
   <si>
     <t>Sparten</t>
-  </si>
-  <si>
-    <t>Dennymane</t>
   </si>
   <si>
     <t>Shimhyangje</t>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="2">
-        <v>46047.57944444445</v>
+        <v>46047.33054398148</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -1784,28 +1784,28 @@
         <v>107</v>
       </c>
       <c r="E22">
-        <v>376</v>
+        <v>354</v>
       </c>
       <c r="F22">
-        <v>336</v>
+        <v>354</v>
       </c>
       <c r="G22">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H22" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I22" t="s">
         <v>154</v>
       </c>
       <c r="J22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K22" t="s">
         <v>155</v>
       </c>
       <c r="L22">
-        <v>805</v>
+        <v>784</v>
       </c>
       <c r="M22" t="s">
         <v>117</v>
@@ -1816,7 +1816,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="2">
-        <v>46047.33054398148</v>
+        <v>46032.86646990741</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
@@ -1828,19 +1828,19 @@
         <v>107</v>
       </c>
       <c r="E23">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="F23">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="G23">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="H23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J23" t="s">
         <v>155</v>
@@ -1849,7 +1849,7 @@
         <v>155</v>
       </c>
       <c r="L23">
-        <v>784</v>
+        <v>798</v>
       </c>
       <c r="M23" t="s">
         <v>118</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="2">
-        <v>46032.86646990741</v>
+        <v>46047.74747685185</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
@@ -1872,28 +1872,28 @@
         <v>107</v>
       </c>
       <c r="E24">
-        <v>361</v>
+        <v>376</v>
       </c>
       <c r="F24">
-        <v>361</v>
+        <v>336</v>
       </c>
       <c r="G24">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="H24" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="I24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K24" t="s">
         <v>155</v>
       </c>
       <c r="L24">
-        <v>798</v>
+        <v>805</v>
       </c>
       <c r="M24" t="s">
         <v>119</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="2">
-        <v>46044.99524305556</v>
+        <v>46045.00385416667</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -2320,19 +2320,19 @@
         <v>112</v>
       </c>
       <c r="E35">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="F35">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="G35">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="H35" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="I35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J35" t="s">
         <v>154</v>
@@ -2341,12 +2341,12 @@
         <v>155</v>
       </c>
       <c r="L35">
-        <v>860</v>
+        <v>847</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="2">
-        <v>46040.06761574074</v>
+        <v>46044.99524305556</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
@@ -2358,16 +2358,16 @@
         <v>112</v>
       </c>
       <c r="E36">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="F36">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="G36">
-        <v>352</v>
+        <v>465</v>
       </c>
       <c r="H36" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="I36" t="s">
         <v>154</v>
@@ -2379,12 +2379,12 @@
         <v>155</v>
       </c>
       <c r="L36">
-        <v>742</v>
+        <v>860</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="2">
-        <v>46026.35682870371</v>
+        <v>46040.06761574074</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
@@ -2396,16 +2396,16 @@
         <v>112</v>
       </c>
       <c r="E37">
-        <v>373</v>
+        <v>390</v>
       </c>
       <c r="F37">
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="G37">
-        <v>451</v>
+        <v>352</v>
       </c>
       <c r="H37" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="I37" t="s">
         <v>154</v>
@@ -2417,12 +2417,12 @@
         <v>155</v>
       </c>
       <c r="L37">
-        <v>826</v>
+        <v>742</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="2">
-        <v>46045.00385416667</v>
+        <v>46026.35682870371</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
@@ -2434,19 +2434,19 @@
         <v>112</v>
       </c>
       <c r="E38">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="F38">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="G38">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="H38" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="I38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J38" t="s">
         <v>154</v>
@@ -2455,7 +2455,7 @@
         <v>155</v>
       </c>
       <c r="L38">
-        <v>847</v>
+        <v>826</v>
       </c>
     </row>
     <row r="39" spans="1:12">

</xml_diff>